<commit_message>
Add Streamlit dashboard with login and GitHub commit fetch
</commit_message>
<xml_diff>
--- a/webapp/src/uploads/predicted_commits_from_github.xlsx
+++ b/webapp/src/uploads/predicted_commits_from_github.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,22 +448,34 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Update README.md with full project description and usage</t>
+          <t>Enhancement: Added GitHub commit fetch + integrated backend logic</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>refactor</t>
+          <t>feature</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Update README.md with full project description and usage</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>refactor</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>Initial commit: DevInsight AI v1 - commit classification and Flask UI</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>feature</t>
         </is>

</xml_diff>